<commit_message>
Features, models and predictions
</commit_message>
<xml_diff>
--- a/data/raw/SinEtiquetatest_cat_6716.xlsx
+++ b/data/raw/SinEtiquetatest_cat_6716.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mavillam\Documents\BIETL\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/ds_ortiz_uniandes_edu_co/Documents/Uniandes/Uniandes/202320 Noveno Semestre/Inteligencia de Negocios/BI-Proyecto-I-Etapa-I/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{900CA330-4D4F-4DD0-A1D4-465AC62C69F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{900CA330-4D4F-4DD0-A1D4-465AC62C69F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3330,9 +3330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B981"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B981"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8250,26 +8248,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8efacf54-3af5-4846-9aca-6e8169fe1a0e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="aea3a4dd-ad68-4c09-8fcd-d380badf67b5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F7B2620488C365419ACDBBCCE69988B8" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b0241bbdfde358bcbfc077e81ce4c5d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8efacf54-3af5-4846-9aca-6e8169fe1a0e" xmlns:ns3="aea3a4dd-ad68-4c09-8fcd-d380badf67b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3c8f9a73de53b87d8956e6923f91fa6" ns2:_="" ns3:_="">
     <xsd:import namespace="8efacf54-3af5-4846-9aca-6e8169fe1a0e"/>
@@ -8518,32 +8496,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96D6DBE9-1D08-48AC-8781-3D469A296AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="aea3a4dd-ad68-4c09-8fcd-d380badf67b5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8efacf54-3af5-4846-9aca-6e8169fe1a0e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22611D1A-AC66-4249-9C13-C425B73FCD28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8efacf54-3af5-4846-9aca-6e8169fe1a0e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="aea3a4dd-ad68-4c09-8fcd-d380badf67b5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1338D932-17F2-4390-BFBD-4AB1467AF0D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8560,4 +8533,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22611D1A-AC66-4249-9C13-C425B73FCD28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96D6DBE9-1D08-48AC-8781-3D469A296AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="aea3a4dd-ad68-4c09-8fcd-d380badf67b5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8efacf54-3af5-4846-9aca-6e8169fe1a0e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>